<commit_message>
added resume upload and retreive it to the CIR in excel
</commit_message>
<xml_diff>
--- a/ExcelTemplate/Book11.xlsx
+++ b/ExcelTemplate/Book11.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17540"/>
+    <workbookView windowWidth="30220" windowHeight="15640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>rollno</t>
   </si>
@@ -42,15 +42,6 @@
   <si>
     <t>gender</t>
   </si>
-  <si>
-    <t>m1372</t>
-  </si>
-  <si>
-    <t>cse</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
 </sst>
 </file>
 
@@ -85,30 +76,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -116,7 +160,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -137,85 +181,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,13 +229,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,19 +349,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +373,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,133 +385,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,26 +426,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -475,31 +463,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,17 +497,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,148 +525,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1011,7 +1002,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1055,35 +1046,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>7.76</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>440</v>
-      </c>
-      <c r="G2">
-        <v>445</v>
-      </c>
-      <c r="H2">
-        <v>2019</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="19" spans="9:9">
       <c r="I19" s="1"/>
     </row>

</xml_diff>